<commit_message>
updating hydrogen UGS costs ans specs
  correcting units and adding AFC
</commit_message>
<xml_diff>
--- a/SubRes_Tmpl/SubRES_NewHydrogen_Trans.xlsx
+++ b/SubRes_Tmpl/SubRES_NewHydrogen_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\Veda_models\IEMM_v60_10-1-master\SubRes_Tmpl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SubRes_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2CE89A-1E62-484A-A1B4-7F1FA0D64D87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A480EBB-36F4-4EFD-9F22-8AD779493F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVA" sheetId="18" r:id="rId1"/>
@@ -61,6 +61,7 @@
   <authors>
     <author>Maurizio Gargiulo</author>
     <author>Gary Goldstein</author>
+    <author>Mahmoud Mobir</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
@@ -103,20 +104,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Insert Table</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="G13" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
@@ -143,12 +130,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="D15" authorId="2" shapeId="0" xr:uid="{2C132A6D-56E2-47CE-A5B1-AF6449975448}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mahmoud Mobir:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+12-21-2021
+Limiting the annual AF to the existing cap</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -211,13 +223,25 @@
   </si>
   <si>
     <t>AFR</t>
+  </si>
+  <si>
+    <t>AFC</t>
+  </si>
+  <si>
+    <t>STH2SUG</t>
+  </si>
+  <si>
+    <t>Other_Indexes</t>
+  </si>
+  <si>
+    <t>ACT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -271,6 +295,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -672,21 +709,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
@@ -696,7 +733,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
@@ -732,36 +769,39 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B3:N14"/>
+  <dimension ref="B3:N15"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -774,7 +814,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="2:14" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -815,7 +855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="E7" s="8"/>
@@ -827,7 +867,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
@@ -840,7 +880,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
@@ -863,7 +903,7 @@
         <v>7</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>8</v>
@@ -879,6 +919,20 @@
       </c>
       <c r="N14" s="5" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -898,27 +952,27 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
     <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>18</v>
       </c>

</xml_diff>